<commit_message>
Ajout du programme et CTE corrigé
le programme qui était déja dans Git hub je l'ai mis dans un dossier 3
oct 2015 parce que je savais pas s'il y avait des modifications que je
n'avais pas
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 4/Documentation/Analyse/P04-JE.xlsx
+++ b/Sprint 1/Package 4/Documentation/Analyse/P04-JE.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Utilisateur\Dropbox\Projet\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18390" windowHeight="6615" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18396" windowHeight="6612" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tblTypeStatus" sheetId="1" r:id="rId1"/>
     <sheet name="tblTypeTest" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,9 +160,6 @@
     <t>Playtests sur prototypes papier</t>
   </si>
   <si>
-    <t>Construire un prototype papier du jeu et le tester avec plusieur joueur et un modérateur qui s'assure que les joueurs sont pas perdu. Analyser les retours des joueur et leurs action en jeu</t>
-  </si>
-  <si>
     <t>PlSce</t>
   </si>
   <si>
@@ -220,6 +212,9 @@
   </si>
   <si>
     <t>Passer en revue les différents actes et séquences constitutifs de la progression du joueur dans la trame narrative</t>
+  </si>
+  <si>
+    <t>Construire un prototype papier du jeu et le tester avec plusieurs joueurs et un modérateur qui s'assure que les joueurs ne sont pas perdus. Analyser les retours des joueurs et leurs actions en jeu.</t>
   </si>
 </sst>
 </file>
@@ -560,7 +555,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -574,11 +569,11 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="82.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="82.33203125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -601,7 +596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -609,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -620,7 +615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -638,16 +633,16 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" customWidth="1"/>
-    <col min="3" max="3" width="94.28515625" customWidth="1"/>
-    <col min="4" max="4" width="162.85546875" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="3" max="3" width="94.33203125" customWidth="1"/>
+    <col min="4" max="4" width="168.109375" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -667,7 +662,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -681,7 +676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -695,7 +690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -709,7 +704,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -723,7 +718,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -737,7 +732,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -754,7 +749,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -765,7 +760,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -776,7 +771,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -784,73 +779,73 @@
         <v>45</v>
       </c>
       <c r="D10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>54</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>57</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>60</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>62</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>63</v>
-      </c>
-      <c r="D16" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>